<commit_message>
My personal information page and tests
</commit_message>
<xml_diff>
--- a/data/projekat.xlsx
+++ b/data/projekat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="TSu2" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="TSu3" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="TSu4" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="TSu5" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="220">
   <si>
     <t xml:space="preserve">Selection</t>
   </si>
@@ -71,7 +72,7 @@
     <t xml:space="preserve">Verify that the user cannot create account if  email is invalid</t>
   </si>
   <si>
-    <t xml:space="preserve">SingIn</t>
+    <t xml:space="preserve">Sign In</t>
   </si>
   <si>
     <t xml:space="preserve">TSu2</t>
@@ -80,28 +81,28 @@
     <t xml:space="preserve">TC4</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user can sing in with valid credentials</t>
+    <t xml:space="preserve">Verify that user can sign in with valid credentials</t>
   </si>
   <si>
     <t xml:space="preserve">TC5</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user can sing in with invalid password</t>
+    <t xml:space="preserve">Verify that user can sign in with invalid password</t>
   </si>
   <si>
     <t xml:space="preserve">TC6</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user can sing in with invalid email address</t>
+    <t xml:space="preserve">Verify that user can sign in with invalid email address</t>
   </si>
   <si>
     <t xml:space="preserve">TC7</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user can sing in with empty credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingOut</t>
+    <t xml:space="preserve">Verify that user can sign in with empty credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign Out</t>
   </si>
   <si>
     <t xml:space="preserve">TSu3</t>
@@ -110,7 +111,7 @@
     <t xml:space="preserve">TC8</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user can sing out</t>
+    <t xml:space="preserve">Verify that user can sign out</t>
   </si>
   <si>
     <t xml:space="preserve">My Address</t>
@@ -137,6 +138,48 @@
     <t xml:space="preserve">Verify that user can deletion address</t>
   </si>
   <si>
+    <t xml:space="preserve">My Personall Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSu5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that only one radio button can be checked at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can leave empty  first name fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can leave empty last name fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can change the date of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that  the user can save the personal information if he does not enter the password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that  the user can save the information if he does enter the invalid password</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test case name: Verify that user can create account with valid email address</t>
   </si>
   <si>
@@ -344,7 +387,7 @@
     <t xml:space="preserve">it is not possible to create an account if you enter the wrong email format</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name:Verify that user can sing in with valid credentials</t>
+    <t xml:space="preserve">Test case name:Verify that user can sign in with valid credentials</t>
   </si>
   <si>
     <t xml:space="preserve">Started Google Chrome Version 89.0.4389.114 (Official Build) (64-bit)</t>
@@ -353,7 +396,7 @@
     <t xml:space="preserve">Navigation to: </t>
   </si>
   <si>
-    <t xml:space="preserve">Click on “Sing in” on menu navigation</t>
+    <t xml:space="preserve">Click on “Sign in” on menu navigation</t>
   </si>
   <si>
     <t xml:space="preserve">Email is entered and visible</t>
@@ -362,13 +405,16 @@
     <t xml:space="preserve">Click to button “Sign in”</t>
   </si>
   <si>
-    <t xml:space="preserve">The user has successfylly sing in</t>
+    <t xml:space="preserve">The user has successfylly sign in</t>
   </si>
   <si>
     <t xml:space="preserve">Sign out</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name:Verify that user can sing in with invalid password</t>
+    <t xml:space="preserve">Test case name:Verify that user can sign in with invalid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation to page from sign in</t>
   </si>
   <si>
     <t xml:space="preserve">S123456789#</t>
@@ -380,25 +426,25 @@
     <t xml:space="preserve">Authentication failed.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name:Verify that user can sing in with invalid email address</t>
+    <t xml:space="preserve">Test case name:Verify that user can sign in with invalid email address</t>
   </si>
   <si>
     <t xml:space="preserve">sanelarajic@gmail</t>
   </si>
   <si>
-    <t xml:space="preserve">The user cannot sing in because the email is not valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test case name:Verify that user can sing in with empty credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user cannot sing in because he has not entered the data</t>
+    <t xml:space="preserve">The user cannot sign in because the email is not valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name:Verify that user can sign in with empty credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user cannot sign in because he has not entered the data</t>
   </si>
   <si>
     <t xml:space="preserve">An email address required.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name: Verify that user can sing out</t>
+    <t xml:space="preserve">Test case name: Verify that user can sign out</t>
   </si>
   <si>
     <t xml:space="preserve">Started Google Chrome Version 89.0.4389.114 (Official Build) (64-bit)   Navigation to: </t>
@@ -407,7 +453,7 @@
     <t xml:space="preserve">Click to button “Sign out”</t>
   </si>
   <si>
-    <t xml:space="preserve">The user has successfylly sing out</t>
+    <t xml:space="preserve">The user has successfylly sign out</t>
   </si>
   <si>
     <t xml:space="preserve">Sign in</t>
@@ -420,6 +466,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Test case name: </t>
     </r>
@@ -438,7 +485,7 @@
     <t xml:space="preserve">Started Google Chrome Version 89.0.4389.114 (Official Build) (64-bit) Navigation to: http://automationpractice.com/index.php                               TC4 PASSED</t>
   </si>
   <si>
-    <t xml:space="preserve">Sing in with valid credentials </t>
+    <t xml:space="preserve">Sign in with valid credentials </t>
   </si>
   <si>
     <t xml:space="preserve">Click on button “My address”</t>
@@ -481,6 +528,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Test case name: </t>
     </r>
@@ -548,6 +596,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Test case name: </t>
     </r>
@@ -568,6 +617,135 @@
   <si>
     <t xml:space="preserve">The user successfully deleted the address </t>
   </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that only one radio button can be checked at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “My personal informaion” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation to “My personal inforamion” page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “Mr.” radio button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radio button “Mr” is checked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “Mrs.” radio button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Mr” radio button is unchecked and “Mrs” radio button is checked </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs check box checked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr check box checked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that user can leave empty  first name fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigg in with valid credentials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “My personal information” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation to “My personal information” page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear the “First name” field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field to “First name” is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Save” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user cannot save changes if the “First name” field is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstname is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that user can leave empty last name fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear the “Lirst name” field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field to “Lirst name” is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user cannot save changes if the “Lirst name” field is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastname is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that the user can change the date of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the day of birthday on drop-down menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day of birthday is change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the mounth of birthday on drop-down menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mounth of birthday is change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the year of birthday on drop-down menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year of birthday is change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user has successfully changed the date of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your personal information has been successfully updated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that  the user can save the personal information if he does not enter the password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field to “Password” is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user cannot save changes if the “Password” field is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The password you entered is incorrect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that  the user can save the information if he does enter the invalid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started Google Chrome Version 89.0.4389.114 (Official Build) (64-bit) Navigation to: http://automationpractice.com/index.php                                                                                                                  TC4 PASSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanela1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user cannot save changes if he has entered invalid password</t>
+  </si>
 </sst>
 </file>
 
@@ -577,7 +755,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -627,16 +805,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -803,7 +977,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="89">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1080,14 +1254,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1116,63 +1282,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1253,20 +1411,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="66.9642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="86.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,6 +1465,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1318,6 +1478,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1419,6 +1581,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1430,6 +1594,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
       <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1437,6 +1603,78 @@
         <v>36</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1464,12 +1702,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="76.4132653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="40.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="67.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="74.6479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="66.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,35 +1715,37 @@
         <v>8</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="9"/>
+      <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>40</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="14" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="15"/>
@@ -1516,11 +1756,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="19" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,13 +1768,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,11 +1782,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="21" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,13 +1794,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1568,13 +1808,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1582,13 +1822,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,13 +1836,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,13 +1850,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D12" s="18" t="n">
         <v>31</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,13 +1864,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,13 +1878,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D14" s="18" t="n">
         <v>1990</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,13 +1892,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,13 +1906,13 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,13 +1920,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,13 +1934,13 @@
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,13 +1948,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,13 +1962,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D20" s="18" t="n">
         <v>21000</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,13 +1976,13 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,13 +1990,13 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,13 +2004,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,11 +2018,11 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="21" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,26 +2031,40 @@
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
     </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+    </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
+      <c r="E28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>40</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="12"/>
@@ -1820,14 +2074,14 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="14" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,11 +2089,11 @@
         <v>1</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="19" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,11 +2101,11 @@
         <v>2</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="D33" s="35"/>
       <c r="E33" s="24" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,11 +2113,11 @@
         <v>3</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D34" s="35"/>
       <c r="E34" s="24" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,33 +2135,53 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="38"/>
       <c r="C37" s="25" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E37" s="40"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
+      <c r="E41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>40</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="12"/>
@@ -1917,14 +2191,14 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="14" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C44" s="32"/>
       <c r="D44" s="7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,11 +2206,11 @@
         <v>1</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D45" s="34"/>
       <c r="E45" s="19" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,13 +2218,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,11 +2232,11 @@
         <v>3</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D47" s="35"/>
       <c r="E47" s="24" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,33 +2254,47 @@
     <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="38"/>
       <c r="C50" s="25" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="E50" s="40"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0"/>
+      <c r="C52" s="0"/>
+      <c r="D52" s="0"/>
+      <c r="E52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
+      <c r="E53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>40</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="12"/>
@@ -2016,14 +2304,14 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="14" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C56" s="32"/>
       <c r="D56" s="7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2031,11 +2319,11 @@
         <v>1</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D57" s="34"/>
       <c r="E57" s="19" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,13 +2331,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="D58" s="41" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,11 +2345,11 @@
         <v>3</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D59" s="35"/>
       <c r="E59" s="24" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,10 +2367,10 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="38"/>
       <c r="C62" s="25" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D62" s="39" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E62" s="40"/>
     </row>
@@ -2115,24 +2403,24 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="62.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="60.4744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.0102040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="61.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="60.7448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="58.9897959183674"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="59.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,7 +2428,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="43"/>
@@ -2155,10 +2443,10 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="44" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="47"/>
@@ -2173,10 +2461,10 @@
       <c r="A3" s="0"/>
       <c r="B3" s="17"/>
       <c r="C3" s="48" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E3" s="47"/>
       <c r="F3" s="0"/>
@@ -2202,14 +2490,14 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="54" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C5" s="55"/>
       <c r="D5" s="56" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F5" s="57"/>
       <c r="G5" s="57"/>
@@ -2224,11 +2512,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="19" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="58"/>
@@ -2243,13 +2531,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="60"/>
@@ -2264,13 +2552,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F8" s="0"/>
       <c r="G8" s="58"/>
@@ -2285,11 +2573,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="21" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="F9" s="58"/>
       <c r="G9" s="58"/>
@@ -2328,10 +2616,10 @@
       <c r="A12" s="0"/>
       <c r="B12" s="12"/>
       <c r="C12" s="25" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D12" s="61" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="E12" s="62"/>
       <c r="F12" s="63"/>
@@ -2360,7 +2648,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="43"/>
@@ -2369,10 +2657,10 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D16" s="46"/>
       <c r="E16" s="0"/>
@@ -2381,10 +2669,10 @@
       <c r="A17" s="0"/>
       <c r="B17" s="17"/>
       <c r="C17" s="4" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E17" s="0"/>
     </row>
@@ -2398,14 +2686,14 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="54" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="56" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2414,11 +2702,11 @@
         <v>1</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="19" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,13 +2715,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D21" s="66" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,13 +2730,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,11 +2745,11 @@
         <v>4</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="21" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,10 +2770,10 @@
       <c r="A26" s="0"/>
       <c r="B26" s="12"/>
       <c r="C26" s="25" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="E26" s="67"/>
     </row>
@@ -2508,7 +2796,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="43"/>
@@ -2517,10 +2805,10 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="44" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D30" s="46"/>
       <c r="E30" s="0"/>
@@ -2529,10 +2817,10 @@
       <c r="A31" s="0"/>
       <c r="B31" s="17"/>
       <c r="C31" s="48" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E31" s="0"/>
     </row>
@@ -2546,14 +2834,14 @@
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="54" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C33" s="55"/>
       <c r="D33" s="56" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,11 +2850,11 @@
         <v>1</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="19" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2575,13 +2863,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D35" s="68" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,13 +2878,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,11 +2893,11 @@
         <v>4</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="21" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,12 +2916,12 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="71" t="s">
-        <v>97</v>
+      <c r="B40" s="50"/>
+      <c r="C40" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="69" t="s">
+        <v>111</v>
       </c>
       <c r="E40" s="67"/>
     </row>
@@ -2656,7 +2944,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="43"/>
@@ -2664,21 +2952,21 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="44" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D44" s="46"/>
       <c r="E44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="17"/>
-      <c r="C45" s="72" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="73" t="s">
-        <v>40</v>
+      <c r="C45" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" s="71" t="s">
+        <v>54</v>
       </c>
       <c r="E45" s="0"/>
     </row>
@@ -2690,14 +2978,14 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="54" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C47" s="55"/>
       <c r="D47" s="56" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E47" s="54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,11 +2993,11 @@
         <v>1</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D48" s="32"/>
       <c r="E48" s="19" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,11 +3005,11 @@
         <v>2</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D49" s="68"/>
       <c r="E49" s="21" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2729,11 +3017,11 @@
         <v>3</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2741,11 +3029,11 @@
         <v>4</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="21" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,14 +3049,14 @@
       <c r="E53" s="15"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="69"/>
-      <c r="C54" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="D54" s="74" t="s">
-        <v>123</v>
-      </c>
-      <c r="E54" s="75"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="E54" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2795,54 +3083,56 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.2908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="51.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="70.6020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="74"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="61.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="78" t="s">
-        <v>125</v>
+        <v>52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>40</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="17"/>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="79"/>
+        <v>57</v>
+      </c>
+      <c r="C4" s="76"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
     </row>
@@ -2850,12 +3140,12 @@
       <c r="B5" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="80" t="s">
-        <v>109</v>
+      <c r="C5" s="77" t="s">
+        <v>123</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="19" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,13 +3153,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2877,54 +3167,54 @@
         <v>3</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="80" t="s">
-        <v>111</v>
+      <c r="C8" s="77" t="s">
+        <v>125</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="80" t="s">
-        <v>126</v>
+      <c r="C9" s="77" t="s">
+        <v>141</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="75"/>
-      <c r="C10" s="81"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="30"/>
       <c r="C11" s="25" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" s="75"/>
+        <v>143</v>
+      </c>
+      <c r="E11" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2950,379 +3240,443 @@
   </sheetPr>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.015306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="70.9948979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.8724489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="69.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="82" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="50.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="85"/>
+      <c r="A2" s="0"/>
+      <c r="B2" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
+      <c r="A3" s="0"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="86" t="s">
-        <v>43</v>
-      </c>
+      <c r="A4" s="0"/>
+      <c r="B4" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="0"/>
       <c r="D4" s="56" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
       <c r="B5" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
       <c r="B6" s="17" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="21" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
       <c r="B7" s="17" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
       <c r="B8" s="17" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
       <c r="B9" s="17" t="n">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
       <c r="B10" s="17" t="n">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
       <c r="B11" s="21"/>
+      <c r="C11" s="0"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
       <c r="B12" s="25"/>
-      <c r="C12" s="87" t="s">
-        <v>96</v>
+      <c r="C12" s="81" t="s">
+        <v>110</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="75"/>
+        <v>157</v>
+      </c>
+      <c r="E12" s="73"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="88"/>
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="83"/>
+      <c r="B16" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="79"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" s="85"/>
+      <c r="A17" s="0"/>
+      <c r="B17" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="58"/>
+      <c r="E17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="89"/>
-      <c r="C18" s="89"/>
+      <c r="A18" s="0"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
       <c r="B19" s="54" t="s">
-        <v>43</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C19" s="0"/>
       <c r="D19" s="56" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
       <c r="B20" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
       <c r="B21" s="17" t="n">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="21" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
       <c r="B22" s="17" t="n">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0"/>
       <c r="B23" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="C23" s="90" t="s">
-        <v>138</v>
+      <c r="C23" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
       <c r="B24" s="17" t="n">
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
       <c r="B25" s="17" t="n">
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
       <c r="B26" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="C26" s="90" t="s">
-        <v>151</v>
+      <c r="C26" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
       <c r="B27" s="17" t="n">
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" s="91" t="s">
-        <v>154</v>
+        <v>168</v>
+      </c>
+      <c r="D27" s="83" t="s">
+        <v>169</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
       <c r="B28" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="C28" s="90" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="91" t="s">
-        <v>85</v>
+      <c r="C28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="83" t="s">
+        <v>99</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
       <c r="B29" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="C29" s="90" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="91" t="s">
-        <v>156</v>
+      <c r="C29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="83" t="s">
+        <v>171</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
       <c r="B30" s="17" t="n">
         <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
       <c r="B31" s="25"/>
       <c r="C31" s="25" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="D31" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="E31" s="75"/>
+      <c r="E31" s="73"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="88"/>
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="92" t="s">
-        <v>159</v>
-      </c>
-      <c r="C34" s="92"/>
-      <c r="D34" s="83"/>
+      <c r="B34" s="84" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="84"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="85"/>
+      <c r="B35" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="58"/>
       <c r="E35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="0"/>
       <c r="E36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="86" t="s">
-        <v>43</v>
-      </c>
+      <c r="B37" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="0"/>
       <c r="D37" s="56" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E37" s="54" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,11 +3684,11 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3342,11 +3696,11 @@
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="D39" s="68"/>
       <c r="E39" s="21" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,32 +3708,34 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="4" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="17"/>
+      <c r="C41" s="0"/>
       <c r="D41" s="21"/>
       <c r="E41" s="21"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="21"/>
+      <c r="C42" s="0"/>
       <c r="D42" s="21"/>
       <c r="E42" s="21"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="25"/>
       <c r="C43" s="25" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="D43" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="E43" s="75"/>
+      <c r="E43" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3395,4 +3751,883 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E111"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D90" activeCellId="0" sqref="D90"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.8316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="85"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="68"/>
+      <c r="E6" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="81" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="73"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="30"/>
+      <c r="C13" s="81" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="87" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="79" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="79"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
+      <c r="B16" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="58"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+      <c r="B19" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="68"/>
+      <c r="E20" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="24" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="73"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="E27" s="25"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="58"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="79" t="s">
+        <v>198</v>
+      </c>
+      <c r="C30" s="79"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="58"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="68"/>
+      <c r="E35" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D38" s="21"/>
+      <c r="E38" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="17"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="17"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="21"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="25"/>
+      <c r="C42" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="88" t="s">
+        <v>202</v>
+      </c>
+      <c r="E42" s="73"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="58"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="79" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" s="79"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="58"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E48" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D50" s="68"/>
+      <c r="E50" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="83" t="n">
+        <v>5</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" s="83" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" s="22" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="21"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+    </row>
+    <row r="57" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="25"/>
+      <c r="C57" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E57" s="73"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="85" t="s">
+        <v>212</v>
+      </c>
+      <c r="C60" s="85"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2"/>
+      <c r="B61" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C61" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D61" s="58"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2"/>
+      <c r="B63" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E63" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2"/>
+      <c r="B64" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2"/>
+      <c r="B65" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" s="68"/>
+      <c r="E65" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2"/>
+      <c r="B66" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2"/>
+      <c r="B67" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+    </row>
+    <row r="71" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" s="25"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="58"/>
+    </row>
+    <row r="74" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="85" t="s">
+        <v>216</v>
+      </c>
+      <c r="C74" s="85"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2"/>
+      <c r="B75" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="D75" s="58"/>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2"/>
+      <c r="B76" s="50"/>
+      <c r="C76" s="50"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2"/>
+      <c r="B77" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E77" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2"/>
+      <c r="B78" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D78" s="21"/>
+      <c r="E78" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2"/>
+      <c r="B79" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" s="68"/>
+      <c r="E79" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2"/>
+      <c r="B80" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2"/>
+      <c r="B81" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D81" s="21"/>
+      <c r="E81" s="24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="73"/>
+    </row>
+    <row r="85" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="E85" s="25"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="167.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B74:C74"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
My wishlist page and tests
</commit_message>
<xml_diff>
--- a/data/projekat.xlsx
+++ b/data/projekat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="TSu3" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="TSu4" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="TSu5" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="TSu6" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="244">
   <si>
     <t xml:space="preserve">Selection</t>
   </si>
@@ -63,13 +64,13 @@
     <t xml:space="preserve">TC2</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that the user cannot create account if  email is not entered</t>
+    <t xml:space="preserve">Verify that user cannot create account if  email is not entered</t>
   </si>
   <si>
     <t xml:space="preserve">TC3</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that the user cannot create account if  email is invalid</t>
+    <t xml:space="preserve">Verify that  user cannot create account if  email is invalid</t>
   </si>
   <si>
     <t xml:space="preserve">Sign In</t>
@@ -171,7 +172,7 @@
     <t xml:space="preserve">TC16</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that  the user can save the personal information if he does not enter the password</t>
+    <t xml:space="preserve">Verify that user can save the personal information if he does not enter the password</t>
   </si>
   <si>
     <t xml:space="preserve">TC17</t>
@@ -180,6 +181,30 @@
     <t xml:space="preserve">Verify that  the user can save the information if he does enter the invalid password</t>
   </si>
   <si>
+    <t xml:space="preserve">My Wishlists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSu6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can add a new wish list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can add several wish lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can remove a wish lists</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test case name: Verify that user can create account with valid email address</t>
   </si>
   <si>
@@ -345,7 +370,7 @@
     <t xml:space="preserve">User is registered and forwarded to “My account” page</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name: Verify that the user cannot create account if  email is not entered</t>
+    <t xml:space="preserve">Test case name: Verify that user cannot create account if  email is not entered</t>
   </si>
   <si>
     <t xml:space="preserve">Leave the field for entering the email address </t>
@@ -372,7 +397,7 @@
     <t xml:space="preserve">An account using this email address has already been registered. Please enter a valid password or request a new one.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name: Verify that the user cannot create account if  email is invalid</t>
+    <t xml:space="preserve">Test case name: Verify that user cannot create account if  email is invalid</t>
   </si>
   <si>
     <t xml:space="preserve">Entered invalid email addresses </t>
@@ -696,7 +721,7 @@
     <t xml:space="preserve">lastname is required.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name: Verify that the user can change the date of birth</t>
+    <t xml:space="preserve">Test case name: Verify that user can change the date of birth</t>
   </si>
   <si>
     <t xml:space="preserve">Change the day of birthday on drop-down menu</t>
@@ -723,7 +748,7 @@
     <t xml:space="preserve">Your personal information has been successfully updated.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name: Verify that  the user can save the personal information if he does not enter the password</t>
+    <t xml:space="preserve">Test case name: Verify that user can save the personal information if he does not enter the password</t>
   </si>
   <si>
     <t xml:space="preserve">Field to “Password” is empty</t>
@@ -735,7 +760,7 @@
     <t xml:space="preserve">The password you entered is incorrect.</t>
   </si>
   <si>
-    <t xml:space="preserve">Test case name: Verify that  the user can save the information if he does enter the invalid password</t>
+    <t xml:space="preserve">Test case name: Verify that user can save the information if he does enter the invalid password</t>
   </si>
   <si>
     <t xml:space="preserve">Started Google Chrome Version 89.0.4389.114 (Official Build) (64-bit) Navigation to: http://automationpractice.com/index.php                                                                                                                  TC4 PASSED</t>
@@ -745,6 +770,54 @@
   </si>
   <si>
     <t xml:space="preserve">The user cannot save changes if he has entered invalid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that user can add a new wish list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “My Wishlists” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation to “My wishlists” page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter name of new wish list in “Name” field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MyWishList1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name is entered and visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New wish list is created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible wishlist count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that user can add several wish lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter name of new wishlist in “Name” field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MyWishList2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the name of the next wish list in “Name” field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MyWishList3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that user can remove a wish lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “x” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wish list is delete</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1403,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1411,20 +1484,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="86.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="84.234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,6 +1697,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
       <c r="C14" s="1" t="s">
         <v>41</v>
       </c>
@@ -1635,6 +1710,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
       <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1646,6 +1723,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
       <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
@@ -1657,6 +1736,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
       <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
@@ -1668,6 +1749,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
       <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
@@ -1676,6 +1759,36 @@
       </c>
       <c r="E18" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1696,18 +1809,18 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="74.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="66.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="73.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="64.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1715,7 +1828,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="9"/>
@@ -1723,13 +1836,13 @@
     </row>
     <row r="2" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E2" s="0"/>
     </row>
@@ -1737,15 +1850,15 @@
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="14" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="15"/>
@@ -1756,11 +1869,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="19" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,13 +1881,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,11 +1895,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="21" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,13 +1907,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,13 +1921,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,13 +1935,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,13 +1949,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,13 +1963,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D12" s="18" t="n">
         <v>31</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,13 +1977,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,13 +1991,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D14" s="18" t="n">
         <v>1990</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,13 +2005,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,13 +2019,13 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,13 +2033,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,13 +2047,13 @@
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,13 +2061,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,13 +2075,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D20" s="18" t="n">
         <v>21000</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1976,13 +2089,13 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,13 +2103,13 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,13 +2117,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,11 +2131,11 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="21" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,7 +2161,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
@@ -2056,13 +2169,13 @@
     </row>
     <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E29" s="0"/>
     </row>
@@ -2074,14 +2187,14 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="14" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,11 +2202,11 @@
         <v>1</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="19" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,11 +2214,11 @@
         <v>2</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D33" s="35"/>
       <c r="E33" s="24" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,11 +2226,11 @@
         <v>3</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D34" s="35"/>
       <c r="E34" s="24" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,10 +2248,10 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="38"/>
       <c r="C37" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E37" s="40"/>
     </row>
@@ -2165,7 +2278,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
@@ -2173,13 +2286,13 @@
     </row>
     <row r="42" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E42" s="0"/>
     </row>
@@ -2191,14 +2304,14 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="14" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C44" s="32"/>
       <c r="D44" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,11 +2319,11 @@
         <v>1</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D45" s="34"/>
       <c r="E45" s="19" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,13 +2331,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,11 +2345,11 @@
         <v>3</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D47" s="35"/>
       <c r="E47" s="24" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,10 +2367,10 @@
     <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="38"/>
       <c r="C50" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E50" s="40"/>
     </row>
@@ -2278,7 +2391,7 @@
         <v>13</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
@@ -2286,13 +2399,13 @@
     </row>
     <row r="54" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E54" s="0"/>
     </row>
@@ -2304,14 +2417,14 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="14" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C56" s="32"/>
       <c r="D56" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,11 +2432,11 @@
         <v>1</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D57" s="34"/>
       <c r="E57" s="19" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,13 +2444,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D58" s="41" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,11 +2458,11 @@
         <v>3</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D59" s="35"/>
       <c r="E59" s="24" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,10 +2480,10 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="38"/>
       <c r="C62" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D62" s="39" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E62" s="40"/>
     </row>
@@ -2403,24 +2516,24 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="58.9897959183674"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="59.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="59.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="57.6428571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="62.9081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="58.3163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2428,7 +2541,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="43"/>
@@ -2443,10 +2556,10 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="44" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="47"/>
@@ -2461,10 +2574,10 @@
       <c r="A3" s="0"/>
       <c r="B3" s="17"/>
       <c r="C3" s="48" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E3" s="47"/>
       <c r="F3" s="0"/>
@@ -2490,14 +2603,14 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C5" s="55"/>
       <c r="D5" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F5" s="57"/>
       <c r="G5" s="57"/>
@@ -2512,11 +2625,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="19" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="58"/>
@@ -2531,13 +2644,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="60"/>
@@ -2552,13 +2665,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F8" s="0"/>
       <c r="G8" s="58"/>
@@ -2573,11 +2686,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F9" s="58"/>
       <c r="G9" s="58"/>
@@ -2616,10 +2729,10 @@
       <c r="A12" s="0"/>
       <c r="B12" s="12"/>
       <c r="C12" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D12" s="61" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E12" s="62"/>
       <c r="F12" s="63"/>
@@ -2648,7 +2761,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="43"/>
@@ -2657,10 +2770,10 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D16" s="46"/>
       <c r="E16" s="0"/>
@@ -2669,10 +2782,10 @@
       <c r="A17" s="0"/>
       <c r="B17" s="17"/>
       <c r="C17" s="4" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E17" s="0"/>
     </row>
@@ -2686,14 +2799,14 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,11 +2815,11 @@
         <v>1</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="19" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,13 +2828,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D21" s="66" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,13 +2843,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,11 +2858,11 @@
         <v>4</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="21" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,10 +2883,10 @@
       <c r="A26" s="0"/>
       <c r="B26" s="12"/>
       <c r="C26" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E26" s="67"/>
     </row>
@@ -2796,7 +2909,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="43"/>
@@ -2805,10 +2918,10 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="44" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D30" s="46"/>
       <c r="E30" s="0"/>
@@ -2817,10 +2930,10 @@
       <c r="A31" s="0"/>
       <c r="B31" s="17"/>
       <c r="C31" s="48" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E31" s="0"/>
     </row>
@@ -2834,14 +2947,14 @@
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C33" s="55"/>
       <c r="D33" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,11 +2963,11 @@
         <v>1</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="19" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,13 +2976,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D35" s="68" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2878,13 +2991,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,11 +3006,11 @@
         <v>4</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="21" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2918,10 +3031,10 @@
       <c r="A40" s="0"/>
       <c r="B40" s="50"/>
       <c r="C40" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D40" s="69" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E40" s="67"/>
     </row>
@@ -2944,7 +3057,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="43"/>
@@ -2952,10 +3065,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="44" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D44" s="46"/>
       <c r="E44" s="0"/>
@@ -2963,10 +3076,10 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="17"/>
       <c r="C45" s="70" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D45" s="71" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E45" s="0"/>
     </row>
@@ -2978,14 +3091,14 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C47" s="55"/>
       <c r="D47" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E47" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2993,11 +3106,11 @@
         <v>1</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D48" s="32"/>
       <c r="E48" s="19" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3005,11 +3118,11 @@
         <v>2</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D49" s="68"/>
       <c r="E49" s="21" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,11 +3130,11 @@
         <v>3</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3029,11 +3142,11 @@
         <v>4</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="21" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3051,10 +3164,10 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="50"/>
       <c r="C54" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D54" s="72" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E54" s="73"/>
     </row>
@@ -3088,11 +3201,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="70.6020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="50.6224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="49.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3100,7 +3213,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="74" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C1" s="74"/>
       <c r="D1" s="75"/>
@@ -3108,13 +3221,13 @@
     </row>
     <row r="2" customFormat="false" ht="61.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E2" s="0"/>
     </row>
@@ -3122,15 +3235,15 @@
       <c r="B3" s="17"/>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="21"/>
@@ -3141,11 +3254,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="77" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="19" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,13 +3266,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,13 +3280,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,11 +3294,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="77" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3193,11 +3306,11 @@
         <v>5</v>
       </c>
       <c r="C9" s="77" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3209,10 +3322,10 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="30"/>
       <c r="C11" s="25" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E11" s="73"/>
     </row>
@@ -3240,19 +3353,19 @@
   </sheetPr>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="69.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="67.765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3260,7 +3373,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C1" s="79"/>
       <c r="D1" s="43"/>
@@ -3269,10 +3382,10 @@
     <row r="2" customFormat="false" ht="50.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="0"/>
@@ -3287,14 +3400,14 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,11 +3416,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3316,11 +3429,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="21" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,11 +3442,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3342,11 +3455,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,13 +3468,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,11 +3483,11 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3388,10 +3501,10 @@
       <c r="A12" s="0"/>
       <c r="B12" s="25"/>
       <c r="C12" s="81" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E12" s="73"/>
     </row>
@@ -3421,7 +3534,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C16" s="79"/>
       <c r="D16" s="43"/>
@@ -3430,10 +3543,10 @@
     <row r="17" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C17" s="71" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D17" s="58"/>
       <c r="E17" s="0"/>
@@ -3448,14 +3561,14 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C19" s="0"/>
       <c r="D19" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3464,11 +3577,11 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3477,11 +3590,11 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="21" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3490,11 +3603,11 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3503,13 +3616,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3518,13 +3631,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3533,13 +3646,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3548,13 +3661,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3563,13 +3676,13 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D27" s="83" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3578,13 +3691,13 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D28" s="83" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,13 +3706,13 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D29" s="83" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,18 +3721,18 @@
         <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="25"/>
       <c r="C31" s="25" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D31" s="39" t="n">
         <v>2</v>
@@ -3645,7 +3758,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="84" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C34" s="84"/>
       <c r="D34" s="43"/>
@@ -3653,10 +3766,10 @@
     </row>
     <row r="35" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D35" s="58"/>
       <c r="E35" s="21"/>
@@ -3669,14 +3782,14 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C37" s="0"/>
       <c r="D37" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E37" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3684,11 +3797,11 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,11 +3809,11 @@
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D39" s="68"/>
       <c r="E39" s="21" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,11 +3821,11 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="4" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3730,7 +3843,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="25"/>
       <c r="C43" s="25" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D43" s="39" t="n">
         <v>1</v>
@@ -3760,18 +3873,18 @@
   </sheetPr>
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D90" activeCellId="0" sqref="D90"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3779,7 +3892,7 @@
         <v>39</v>
       </c>
       <c r="B1" s="85" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C1" s="85"/>
       <c r="D1" s="43"/>
@@ -3788,10 +3901,10 @@
     <row r="2" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="1"/>
@@ -3804,14 +3917,14 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,11 +3933,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,11 +3946,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="21" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3846,11 +3959,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3859,11 +3972,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,20 +4004,20 @@
       <c r="A12" s="2"/>
       <c r="B12" s="25"/>
       <c r="C12" s="81" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E12" s="73"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="30"/>
       <c r="C13" s="81" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3912,7 +4025,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="79" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C15" s="79"/>
       <c r="D15" s="43"/>
@@ -3921,10 +4034,10 @@
     <row r="16" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D16" s="58"/>
       <c r="E16" s="1"/>
@@ -3937,14 +4050,14 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3953,11 +4066,11 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3966,11 +4079,11 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="21" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3979,11 +4092,11 @@
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,13 +4105,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,11 +4120,11 @@
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="24" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4039,10 +4152,10 @@
       <c r="A27" s="2"/>
       <c r="B27" s="25"/>
       <c r="C27" s="81" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E27" s="25"/>
     </row>
@@ -4058,7 +4171,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="79" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C30" s="79"/>
       <c r="D30" s="43"/>
@@ -4066,10 +4179,10 @@
     </row>
     <row r="31" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C31" s="71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D31" s="58"/>
       <c r="E31" s="1"/>
@@ -4080,14 +4193,14 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4095,11 +4208,11 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4107,11 +4220,11 @@
         <v>2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D35" s="68"/>
       <c r="E35" s="21" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4119,11 +4232,11 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="21" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,13 +4244,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4145,11 +4258,11 @@
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="4" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4173,12 +4286,12 @@
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="25"/>
       <c r="C42" s="81" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D42" s="88" t="s">
-        <v>202</v>
-      </c>
-      <c r="E42" s="73"/>
+        <v>210</v>
+      </c>
+      <c r="E42" s="25"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
@@ -4192,7 +4305,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="79" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C45" s="79"/>
       <c r="D45" s="43"/>
@@ -4200,10 +4313,10 @@
     </row>
     <row r="46" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D46" s="58"/>
       <c r="E46" s="1"/>
@@ -4214,14 +4327,14 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E48" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,11 +4342,11 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4241,11 +4354,11 @@
         <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D50" s="68"/>
       <c r="E50" s="21" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4253,13 +4366,13 @@
         <v>3</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D51" s="83" t="n">
         <v>5</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4267,13 +4380,13 @@
         <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="D52" s="83" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4281,13 +4394,13 @@
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D53" s="22" t="n">
         <v>2000</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4295,13 +4408,13 @@
         <v>6</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4309,11 +4422,11 @@
         <v>7</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="4" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4325,10 +4438,10 @@
     <row r="57" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="25"/>
       <c r="C57" s="81" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D57" s="39" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="E57" s="73"/>
     </row>
@@ -4338,7 +4451,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="85" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C60" s="85"/>
       <c r="D60" s="43"/>
@@ -4347,10 +4460,10 @@
     <row r="61" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C61" s="71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D61" s="58"/>
       <c r="E61" s="1"/>
@@ -4363,14 +4476,14 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E63" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4379,11 +4492,11 @@
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,11 +4505,11 @@
         <v>2</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D65" s="68"/>
       <c r="E65" s="21" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4405,11 +4518,11 @@
         <v>4</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4418,11 +4531,11 @@
         <v>5</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="4" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4450,10 +4563,10 @@
       <c r="A71" s="2"/>
       <c r="B71" s="25"/>
       <c r="C71" s="81" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D71" s="39" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E71" s="25"/>
     </row>
@@ -4469,7 +4582,7 @@
         <v>47</v>
       </c>
       <c r="B74" s="85" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="C74" s="85"/>
       <c r="D74" s="43"/>
@@ -4478,10 +4591,10 @@
     <row r="75" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
       <c r="B75" s="80" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C75" s="71" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="D75" s="58"/>
       <c r="E75" s="1"/>
@@ -4494,14 +4607,14 @@
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
       <c r="B77" s="54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E77" s="54" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4510,11 +4623,11 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="19" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4523,11 +4636,11 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D79" s="68"/>
       <c r="E79" s="21" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,13 +4649,13 @@
         <v>4</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4551,11 +4664,11 @@
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="24" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4583,10 +4696,10 @@
       <c r="A85" s="2"/>
       <c r="B85" s="25"/>
       <c r="C85" s="81" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D85" s="39" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E85" s="25"/>
     </row>
@@ -4630,4 +4743,432 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="85"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="68"/>
+      <c r="E6" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="81" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="73"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="85" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="85"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
+      <c r="B16" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="58"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+      <c r="B19" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="68"/>
+      <c r="E20" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="81" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="73"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="85" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="85"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="58"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
+      <c r="B35" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D36" s="68"/>
+      <c r="E36" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2"/>
+      <c r="B37" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="81" t="s">
+        <v>235</v>
+      </c>
+      <c r="D41" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B31:C31"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added products tests and pages
</commit_message>
<xml_diff>
--- a/data/projekat.xlsx
+++ b/data/projekat.xlsx
@@ -15,6 +15,7 @@
     <sheet name="TSu4" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="TSu5" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="TSu6" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="TSu7" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="287">
   <si>
     <t xml:space="preserve">Selection</t>
   </si>
@@ -203,6 +204,36 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that user can remove a wish lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding product to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSu7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can addition of one product to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the user can add one product three times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if the user can add  several products to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can remove product from cart</t>
   </si>
   <si>
     <t xml:space="preserve">Test case name: Verify that user can create account with valid email address</t>
@@ -646,6 +677,9 @@
     <t xml:space="preserve">Test case name: Verify that only one radio button can be checked at the same time</t>
   </si>
   <si>
+    <t xml:space="preserve">Started Google Chrome Version 89.0.4389.114 (Official Build) (64-bit) Navigation to: http://automationpractice.com/index.php                            TC4 PASSED</t>
+  </si>
+  <si>
     <t xml:space="preserve">Click on “My personal informaion” button</t>
   </si>
   <si>
@@ -818,6 +852,102 @@
   </si>
   <si>
     <t xml:space="preserve">Wish list is delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that the user  can addition of one product to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sing in with valid credentials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user has successfylly sing in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Woman” tab on menu navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to “Woman” page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Dresses”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to “Dresses” page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “More” about the product  Printed Dress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A product information page has opened</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Add to cart” for dress Printed Dress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We added Printed Dress to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Proceed to checkout”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation to cart and checking the products we added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that if the user can add one product three times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The quantity was changed to three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that if the user can add several products to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Continue shopping”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue to shopping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “More” about the product  Printed Summer Dress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Add to cart” for dress Printed Summer Dress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We added Printed Summer Dress to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “More” about the product Printed Chiffon Dress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Add to cart” for dress Printed Chiffon Dress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We added  to cart Printed Chiffon Dress to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case name: Verify that the user can remove product from cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to “Delate”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the product is deleted from the cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your shopping cart is empty.</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1404,6 +1534,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1484,20 +1622,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="84.234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="82.3469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,21 +1912,84 @@
       <c r="D19" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
       <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
       <c r="C21" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1809,18 +2010,18 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="73.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="64.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="71.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="43.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="63.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,7 +2029,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="9"/>
@@ -1836,13 +2037,13 @@
     </row>
     <row r="2" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E2" s="0"/>
     </row>
@@ -1850,15 +2051,15 @@
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="14" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="15"/>
@@ -1869,11 +2070,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="19" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,13 +2082,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,11 +2096,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="21" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,13 +2108,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,13 +2122,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,13 +2136,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,13 +2150,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,13 +2164,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D12" s="18" t="n">
         <v>31</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,13 +2178,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,13 +2192,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D14" s="18" t="n">
         <v>1990</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,13 +2206,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,13 +2220,13 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,13 +2234,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,13 +2248,13 @@
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,13 +2262,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2075,13 +2276,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D20" s="18" t="n">
         <v>21000</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,13 +2290,13 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,13 +2304,13 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,13 +2318,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,11 +2332,11 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="21" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,7 +2362,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
@@ -2169,13 +2370,13 @@
     </row>
     <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E29" s="0"/>
     </row>
@@ -2187,14 +2388,14 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="14" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,11 +2403,11 @@
         <v>1</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="19" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,11 +2415,11 @@
         <v>2</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D33" s="35"/>
       <c r="E33" s="24" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,11 +2427,11 @@
         <v>3</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D34" s="35"/>
       <c r="E34" s="24" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2248,10 +2449,10 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="38"/>
       <c r="C37" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E37" s="40"/>
     </row>
@@ -2278,7 +2479,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
@@ -2286,13 +2487,13 @@
     </row>
     <row r="42" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E42" s="0"/>
     </row>
@@ -2304,14 +2505,14 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="14" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C44" s="32"/>
       <c r="D44" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,11 +2520,11 @@
         <v>1</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D45" s="34"/>
       <c r="E45" s="19" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,13 +2532,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,11 +2546,11 @@
         <v>3</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D47" s="35"/>
       <c r="E47" s="24" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,10 +2568,10 @@
     <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="38"/>
       <c r="C50" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E50" s="40"/>
     </row>
@@ -2391,7 +2592,7 @@
         <v>13</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
@@ -2399,13 +2600,13 @@
     </row>
     <row r="54" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E54" s="0"/>
     </row>
@@ -2417,14 +2618,14 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="14" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C56" s="32"/>
       <c r="D56" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,11 +2633,11 @@
         <v>1</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D57" s="34"/>
       <c r="E57" s="19" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,13 +2645,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D58" s="41" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,11 +2659,11 @@
         <v>3</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D59" s="35"/>
       <c r="E59" s="24" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,10 +2681,10 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="38"/>
       <c r="C62" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D62" s="39" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E62" s="40"/>
     </row>
@@ -2516,24 +2717,24 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="59.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="57.6428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="62.9081632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="58.3163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.8877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="57.9132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="61.4234693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2541,7 +2742,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="43"/>
@@ -2556,10 +2757,10 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="44" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="47"/>
@@ -2574,10 +2775,10 @@
       <c r="A3" s="0"/>
       <c r="B3" s="17"/>
       <c r="C3" s="48" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E3" s="47"/>
       <c r="F3" s="0"/>
@@ -2603,14 +2804,14 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C5" s="55"/>
       <c r="D5" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="F5" s="57"/>
       <c r="G5" s="57"/>
@@ -2625,11 +2826,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="19" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="58"/>
@@ -2644,13 +2845,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="60"/>
@@ -2665,13 +2866,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F8" s="0"/>
       <c r="G8" s="58"/>
@@ -2686,11 +2887,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="F9" s="58"/>
       <c r="G9" s="58"/>
@@ -2729,10 +2930,10 @@
       <c r="A12" s="0"/>
       <c r="B12" s="12"/>
       <c r="C12" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D12" s="61" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E12" s="62"/>
       <c r="F12" s="63"/>
@@ -2761,7 +2962,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="43"/>
@@ -2770,10 +2971,10 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D16" s="46"/>
       <c r="E16" s="0"/>
@@ -2782,10 +2983,10 @@
       <c r="A17" s="0"/>
       <c r="B17" s="17"/>
       <c r="C17" s="4" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E17" s="0"/>
     </row>
@@ -2799,14 +3000,14 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,11 +3016,11 @@
         <v>1</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="19" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,13 +3029,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D21" s="66" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2843,13 +3044,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,11 +3059,11 @@
         <v>4</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="21" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,10 +3084,10 @@
       <c r="A26" s="0"/>
       <c r="B26" s="12"/>
       <c r="C26" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E26" s="67"/>
     </row>
@@ -2909,7 +3110,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="43"/>
@@ -2918,10 +3119,10 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="44" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D30" s="46"/>
       <c r="E30" s="0"/>
@@ -2930,10 +3131,10 @@
       <c r="A31" s="0"/>
       <c r="B31" s="17"/>
       <c r="C31" s="48" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E31" s="0"/>
     </row>
@@ -2947,14 +3148,14 @@
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C33" s="55"/>
       <c r="D33" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2963,11 +3164,11 @@
         <v>1</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="19" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2976,13 +3177,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D35" s="68" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="21" t="s">
         <v>142</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,13 +3192,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,11 +3207,11 @@
         <v>4</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="21" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3031,10 +3232,10 @@
       <c r="A40" s="0"/>
       <c r="B40" s="50"/>
       <c r="C40" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D40" s="69" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E40" s="67"/>
     </row>
@@ -3057,7 +3258,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="43"/>
@@ -3065,10 +3266,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="44" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D44" s="46"/>
       <c r="E44" s="0"/>
@@ -3076,10 +3277,10 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="17"/>
       <c r="C45" s="70" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D45" s="71" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E45" s="0"/>
     </row>
@@ -3091,14 +3292,14 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C47" s="55"/>
       <c r="D47" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E47" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,11 +3307,11 @@
         <v>1</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D48" s="32"/>
       <c r="E48" s="19" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3118,11 +3319,11 @@
         <v>2</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D49" s="68"/>
       <c r="E49" s="21" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,11 +3331,11 @@
         <v>3</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,11 +3343,11 @@
         <v>4</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="21" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,10 +3365,10 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="50"/>
       <c r="C54" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D54" s="72" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E54" s="73"/>
     </row>
@@ -3201,11 +3402,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.9795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3213,7 +3414,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="74" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C1" s="74"/>
       <c r="D1" s="75"/>
@@ -3221,13 +3422,13 @@
     </row>
     <row r="2" customFormat="false" ht="61.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E2" s="0"/>
     </row>
@@ -3235,15 +3436,15 @@
       <c r="B3" s="17"/>
       <c r="C3" s="4"/>
       <c r="D3" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="10" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="21"/>
@@ -3254,11 +3455,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="77" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="19" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,13 +3467,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3280,13 +3481,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3294,11 +3495,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="77" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,11 +3507,11 @@
         <v>5</v>
       </c>
       <c r="C9" s="77" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3322,10 +3523,10 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="30"/>
       <c r="C11" s="25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="E11" s="73"/>
     </row>
@@ -3353,19 +3554,19 @@
   </sheetPr>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="67.765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="66.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3373,7 +3574,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C1" s="79"/>
       <c r="D1" s="43"/>
@@ -3382,10 +3583,10 @@
     <row r="2" customFormat="false" ht="50.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="0"/>
@@ -3400,14 +3601,14 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,11 +3617,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,11 +3630,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="21" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,11 +3643,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3455,11 +3656,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,13 +3669,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,11 +3684,11 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3501,10 +3702,10 @@
       <c r="A12" s="0"/>
       <c r="B12" s="25"/>
       <c r="C12" s="81" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="E12" s="73"/>
     </row>
@@ -3534,7 +3735,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C16" s="79"/>
       <c r="D16" s="43"/>
@@ -3543,10 +3744,10 @@
     <row r="17" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C17" s="71" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D17" s="58"/>
       <c r="E17" s="0"/>
@@ -3561,14 +3762,14 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C19" s="0"/>
       <c r="D19" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3577,11 +3778,11 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3590,11 +3791,11 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="21" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3603,11 +3804,11 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3616,13 +3817,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,13 +3832,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3646,13 +3847,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3661,13 +3862,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3676,13 +3877,13 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D27" s="83" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,13 +3892,13 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D28" s="83" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3706,13 +3907,13 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D29" s="83" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3721,18 +3922,18 @@
         <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="25"/>
       <c r="C31" s="25" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="D31" s="39" t="n">
         <v>2</v>
@@ -3758,7 +3959,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="84" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C34" s="84"/>
       <c r="D34" s="43"/>
@@ -3766,10 +3967,10 @@
     </row>
     <row r="35" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D35" s="58"/>
       <c r="E35" s="21"/>
@@ -3782,14 +3983,14 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C37" s="0"/>
       <c r="D37" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E37" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3797,11 +3998,11 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,11 +4010,11 @@
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D39" s="68"/>
       <c r="E39" s="21" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3821,11 +4022,11 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="4" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +4044,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="25"/>
       <c r="C43" s="25" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="D43" s="39" t="n">
         <v>1</v>
@@ -3873,18 +4074,18 @@
   </sheetPr>
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.5765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3892,19 +4093,19 @@
         <v>39</v>
       </c>
       <c r="B1" s="85" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="C1" s="85"/>
       <c r="D1" s="43"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="1"/>
@@ -3917,14 +4118,14 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3933,11 +4134,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3946,11 +4147,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="21" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3959,11 +4160,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3972,11 +4173,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4004,20 +4205,20 @@
       <c r="A12" s="2"/>
       <c r="B12" s="25"/>
       <c r="C12" s="81" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="E12" s="73"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="30"/>
       <c r="C13" s="81" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,19 +4226,19 @@
         <v>41</v>
       </c>
       <c r="B15" s="79" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C15" s="79"/>
       <c r="D15" s="43"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="D16" s="58"/>
       <c r="E16" s="1"/>
@@ -4050,14 +4251,14 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4066,11 +4267,11 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4079,11 +4280,11 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="21" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4092,11 +4293,11 @@
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4105,13 +4306,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4120,11 +4321,11 @@
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="24" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4152,10 +4353,10 @@
       <c r="A27" s="2"/>
       <c r="B27" s="25"/>
       <c r="C27" s="81" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="E27" s="25"/>
     </row>
@@ -4171,18 +4372,18 @@
         <v>43</v>
       </c>
       <c r="B30" s="79" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="C30" s="79"/>
       <c r="D30" s="43"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C31" s="71" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="D31" s="58"/>
       <c r="E31" s="1"/>
@@ -4193,14 +4394,14 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4208,11 +4409,11 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,11 +4421,11 @@
         <v>2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="D35" s="68"/>
       <c r="E35" s="21" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4232,11 +4433,11 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="21" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4244,13 +4445,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4258,11 +4459,11 @@
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="4" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,10 +4487,10 @@
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="25"/>
       <c r="C42" s="81" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D42" s="88" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="E42" s="25"/>
     </row>
@@ -4305,18 +4506,18 @@
         <v>45</v>
       </c>
       <c r="B45" s="79" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C45" s="79"/>
       <c r="D45" s="43"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="D46" s="58"/>
       <c r="E46" s="1"/>
@@ -4327,14 +4528,14 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E48" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4342,11 +4543,11 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4354,11 +4555,11 @@
         <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="D50" s="68"/>
       <c r="E50" s="21" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4366,13 +4567,13 @@
         <v>3</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D51" s="83" t="n">
         <v>5</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4380,13 +4581,13 @@
         <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="D52" s="83" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,13 +4595,13 @@
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="D53" s="22" t="n">
         <v>2000</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4408,13 +4609,13 @@
         <v>6</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4422,11 +4623,11 @@
         <v>7</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="4" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4438,10 +4639,10 @@
     <row r="57" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="25"/>
       <c r="C57" s="81" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D57" s="39" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="E57" s="73"/>
     </row>
@@ -4451,19 +4652,19 @@
         <v>47</v>
       </c>
       <c r="B60" s="85" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="C60" s="85"/>
       <c r="D60" s="43"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C61" s="71" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="D61" s="58"/>
       <c r="E61" s="1"/>
@@ -4476,14 +4677,14 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E63" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4492,11 +4693,11 @@
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4505,11 +4706,11 @@
         <v>2</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="D65" s="68"/>
       <c r="E65" s="21" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,11 +4719,11 @@
         <v>4</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4531,11 +4732,11 @@
         <v>5</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="4" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4563,10 +4764,10 @@
       <c r="A71" s="2"/>
       <c r="B71" s="25"/>
       <c r="C71" s="81" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D71" s="39" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="E71" s="25"/>
     </row>
@@ -4582,7 +4783,7 @@
         <v>47</v>
       </c>
       <c r="B74" s="85" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="C74" s="85"/>
       <c r="D74" s="43"/>
@@ -4591,10 +4792,10 @@
     <row r="75" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
       <c r="B75" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C75" s="71" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="D75" s="58"/>
       <c r="E75" s="1"/>
@@ -4607,14 +4808,14 @@
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
       <c r="B77" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E77" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4623,11 +4824,11 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="19" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4636,11 +4837,11 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="D79" s="68"/>
       <c r="E79" s="21" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4649,13 +4850,13 @@
         <v>4</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4664,11 +4865,11 @@
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="24" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4696,10 +4897,10 @@
       <c r="A85" s="2"/>
       <c r="B85" s="25"/>
       <c r="C85" s="81" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D85" s="39" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="E85" s="25"/>
     </row>
@@ -4752,18 +4953,18 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.9795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4771,7 +4972,7 @@
         <v>53</v>
       </c>
       <c r="B1" s="85" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="C1" s="85"/>
       <c r="D1" s="43"/>
@@ -4780,10 +4981,10 @@
     <row r="2" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="1"/>
@@ -4796,14 +4997,14 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4812,11 +5013,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4825,11 +5026,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="D6" s="68"/>
       <c r="E6" s="21" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4838,13 +5039,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4853,11 +5054,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +5086,7 @@
       <c r="A12" s="2"/>
       <c r="B12" s="25"/>
       <c r="C12" s="81" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="D12" s="39" t="n">
         <v>1</v>
@@ -4897,7 +5098,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="85" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="C15" s="85"/>
       <c r="D15" s="43"/>
@@ -4906,10 +5107,10 @@
     <row r="16" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D16" s="58"/>
       <c r="E16" s="1"/>
@@ -4922,14 +5123,14 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4938,11 +5139,11 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4951,11 +5152,11 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="21" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4964,13 +5165,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4979,11 +5180,11 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4992,13 +5193,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5007,11 +5208,11 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5039,7 +5240,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="25"/>
       <c r="C28" s="81" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="D28" s="39" t="n">
         <v>3</v>
@@ -5051,7 +5252,7 @@
         <v>57</v>
       </c>
       <c r="B31" s="85" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="C31" s="85"/>
       <c r="D31" s="43"/>
@@ -5060,10 +5261,10 @@
     <row r="32" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="80" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C32" s="71" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D32" s="58"/>
       <c r="E32" s="1"/>
@@ -5076,14 +5277,14 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="54" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="56" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E34" s="54" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5092,11 +5293,11 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="21" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5105,11 +5306,11 @@
         <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="D36" s="68"/>
       <c r="E36" s="21" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5118,11 +5319,11 @@
         <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="21" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5150,7 +5351,7 @@
       <c r="A41" s="2"/>
       <c r="B41" s="25"/>
       <c r="C41" s="81" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="D41" s="39" t="n">
         <v>2</v>
@@ -5171,4 +5372,769 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E69"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="79"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="68"/>
+      <c r="E6" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="73"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="79" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" s="79"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="58"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+      <c r="B19" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="68"/>
+      <c r="E21" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D22" s="68"/>
+      <c r="E22" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="D23" s="68"/>
+      <c r="E23" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="D24" s="90" t="s">
+        <v>271</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="D25" s="68"/>
+      <c r="E25" s="24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="D26" s="68"/>
+      <c r="E26" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="15"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="73"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="81" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="86" t="s">
+        <v>273</v>
+      </c>
+      <c r="E29" s="25"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="C32" s="79"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
+      <c r="B33" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" s="58"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
+      <c r="B35" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D36" s="21"/>
+      <c r="E36" s="19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2"/>
+      <c r="B37" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="68"/>
+      <c r="E37" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2"/>
+      <c r="B38" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2"/>
+      <c r="B39" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="D39" s="21"/>
+      <c r="E39" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2"/>
+      <c r="B40" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D40" s="21"/>
+      <c r="E40" s="24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+      <c r="B41" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D41" s="21"/>
+      <c r="E41" s="24" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2"/>
+      <c r="B42" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="68"/>
+      <c r="E42" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2"/>
+      <c r="B43" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2"/>
+      <c r="B44" s="17" t="n">
+        <v>9</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D44" s="21"/>
+      <c r="E44" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2"/>
+      <c r="B45" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D45" s="21"/>
+      <c r="E45" s="24" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2"/>
+      <c r="B46" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D46" s="21"/>
+      <c r="E46" s="24" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2"/>
+      <c r="B47" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="68"/>
+      <c r="E47" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2"/>
+      <c r="B48" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2"/>
+      <c r="B49" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2"/>
+      <c r="B50" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2"/>
+      <c r="B51" s="17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2"/>
+      <c r="B52" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="81" t="s">
+        <v>268</v>
+      </c>
+      <c r="D54" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" s="25"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="79" t="s">
+        <v>283</v>
+      </c>
+      <c r="C57" s="79"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2"/>
+      <c r="B58" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="71" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="58"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2"/>
+      <c r="B60" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2"/>
+      <c r="B61" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2"/>
+      <c r="B62" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="68"/>
+      <c r="E62" s="21" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2"/>
+      <c r="B63" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2"/>
+      <c r="B64" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2"/>
+      <c r="B65" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2"/>
+      <c r="B66" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2"/>
+      <c r="B67" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="73"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" s="86" t="s">
+        <v>286</v>
+      </c>
+      <c r="E69" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B57:C57"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>